<commit_message>
Commit more data for ROC curves.
</commit_message>
<xml_diff>
--- a/assignment1/ROC curve data points.xlsx
+++ b/assignment1/ROC curve data points.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{469DF27D-A17C-44CA-85AE-8A3AC535B19C}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{1B31E21A-7F41-4FFA-A057-431E940B83D6}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="108">
   <si>
     <t>TPR and FPR for ROC curves</t>
   </si>
@@ -275,6 +275,75 @@
   </si>
   <si>
     <t>0.1778</t>
+  </si>
+  <si>
+    <t>Weight for malicious traffic</t>
+  </si>
+  <si>
+    <t>0.7143</t>
+  </si>
+  <si>
+    <t>0.9987</t>
+  </si>
+  <si>
+    <t>0.0013</t>
+  </si>
+  <si>
+    <t>0.9989</t>
+  </si>
+  <si>
+    <t>0.001</t>
+  </si>
+  <si>
+    <t>0.8333</t>
+  </si>
+  <si>
+    <t>0.9993</t>
+  </si>
+  <si>
+    <t>0.814</t>
+  </si>
+  <si>
+    <t>0.1924</t>
+  </si>
+  <si>
+    <t>0.0385</t>
+  </si>
+  <si>
+    <t>0.0294</t>
+  </si>
+  <si>
+    <t>0.0432</t>
+  </si>
+  <si>
+    <t>0.0028</t>
+  </si>
+  <si>
+    <t>0.0175</t>
+  </si>
+  <si>
+    <t>0.0083</t>
+  </si>
+  <si>
+    <t>0.0224</t>
+  </si>
+  <si>
+    <t>0.0202</t>
+  </si>
+  <si>
+    <t>0.0481</t>
+  </si>
+  <si>
+    <t>0.0098</t>
+  </si>
+  <si>
+    <t>0.1197</t>
+  </si>
+  <si>
+    <t>0.0053</t>
+  </si>
+  <si>
+    <t>0.254</t>
   </si>
 </sst>
 </file>
@@ -715,10 +784,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:H30"/>
+  <dimension ref="B2:O30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H31" sqref="H31"/>
+      <selection activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -729,9 +798,13 @@
     <col min="5" max="5" width="11.28515625" customWidth="1"/>
     <col min="6" max="6" width="12.7109375" customWidth="1"/>
     <col min="7" max="7" width="11.85546875" customWidth="1"/>
+    <col min="10" max="10" width="31.42578125" customWidth="1"/>
+    <col min="11" max="11" width="26" customWidth="1"/>
+    <col min="12" max="12" width="12" customWidth="1"/>
+    <col min="14" max="14" width="13.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>0</v>
       </c>
@@ -745,8 +818,18 @@
         <v>5</v>
       </c>
       <c r="H2" s="3"/>
-    </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J2" s="1"/>
+      <c r="K2" s="10"/>
+      <c r="L2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="M2" s="3"/>
+      <c r="N2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="O2" s="3"/>
+    </row>
+    <row r="3" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C3" s="7" t="s">
         <v>1</v>
       </c>
@@ -765,8 +848,26 @@
       <c r="H3" s="9" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J3" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="K3" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="L3" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="M3" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="N3" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="O3" s="9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C4" s="4" t="s">
         <v>2</v>
       </c>
@@ -785,8 +886,26 @@
       <c r="H4" s="6" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J4" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="K4" s="2">
+        <v>1</v>
+      </c>
+      <c r="L4" s="2">
+        <v>1</v>
+      </c>
+      <c r="M4" s="2">
+        <v>0</v>
+      </c>
+      <c r="N4" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="O4" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="5" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C5" s="4"/>
       <c r="D5" s="5" t="s">
         <v>7</v>
@@ -803,8 +922,24 @@
       <c r="H5" s="6" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J5" s="4"/>
+      <c r="K5" s="5">
+        <v>5</v>
+      </c>
+      <c r="L5" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="M5" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="N5" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="O5" s="6" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="6" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C6" s="4"/>
       <c r="D6" s="5" t="s">
         <v>8</v>
@@ -821,8 +956,24 @@
       <c r="H6" s="6" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J6" s="4"/>
+      <c r="K6" s="5">
+        <v>10</v>
+      </c>
+      <c r="L6" s="5">
+        <v>1</v>
+      </c>
+      <c r="M6" s="5">
+        <v>0</v>
+      </c>
+      <c r="N6" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="O6" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C7" s="4"/>
       <c r="D7" s="5" t="s">
         <v>9</v>
@@ -839,8 +990,24 @@
       <c r="H7" s="6" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J7" s="4"/>
+      <c r="K7" s="5">
+        <v>25</v>
+      </c>
+      <c r="L7" s="5">
+        <v>1</v>
+      </c>
+      <c r="M7" s="5">
+        <v>0</v>
+      </c>
+      <c r="N7" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="O7" s="6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="8" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C8" s="4"/>
       <c r="D8" s="5" t="s">
         <v>10</v>
@@ -857,8 +1024,24 @@
       <c r="H8" s="6" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J8" s="4"/>
+      <c r="K8" s="5">
+        <v>50</v>
+      </c>
+      <c r="L8" s="12">
+        <v>1</v>
+      </c>
+      <c r="M8" s="12">
+        <v>0</v>
+      </c>
+      <c r="N8" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="O8" s="6" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="9" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C9" s="4"/>
       <c r="D9" s="5" t="s">
         <v>11</v>
@@ -875,8 +1058,24 @@
       <c r="H9" s="6" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J9" s="4"/>
+      <c r="K9" s="5">
+        <v>100</v>
+      </c>
+      <c r="L9" s="12">
+        <v>1</v>
+      </c>
+      <c r="M9" s="12">
+        <v>0</v>
+      </c>
+      <c r="N9" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="O9" s="6" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="10" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C10" s="4"/>
       <c r="D10" s="5" t="s">
         <v>12</v>
@@ -893,8 +1092,24 @@
       <c r="H10" s="6" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J10" s="4"/>
+      <c r="K10" s="5">
+        <v>250</v>
+      </c>
+      <c r="L10" s="12">
+        <v>1</v>
+      </c>
+      <c r="M10" s="12">
+        <v>0</v>
+      </c>
+      <c r="N10" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="O10" s="6" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="11" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C11" s="4"/>
       <c r="D11" s="5" t="s">
         <v>13</v>
@@ -911,8 +1126,24 @@
       <c r="H11" s="6" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J11" s="4"/>
+      <c r="K11" s="5">
+        <v>500</v>
+      </c>
+      <c r="L11" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="M11" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="N11" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="O11" s="6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C12" s="7"/>
       <c r="D12" s="8" t="s">
         <v>14</v>
@@ -929,8 +1160,24 @@
       <c r="H12" s="9" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J12" s="7"/>
+      <c r="K12" s="8">
+        <v>1000</v>
+      </c>
+      <c r="L12" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="M12" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="N12" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="O12" s="9" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="13" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C13" s="1" t="s">
         <v>44</v>
       </c>
@@ -949,8 +1196,26 @@
       <c r="H13" s="15" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J13" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="K13" s="2">
+        <v>1</v>
+      </c>
+      <c r="L13" s="2">
+        <v>0</v>
+      </c>
+      <c r="M13" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="N13" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="O13" s="3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="14" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C14" s="4"/>
       <c r="D14" s="5" t="s">
         <v>7</v>
@@ -967,8 +1232,24 @@
       <c r="H14" s="13" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J14" s="4"/>
+      <c r="K14" s="5">
+        <v>5</v>
+      </c>
+      <c r="L14" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="M14" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="N14" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="O14" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C15" s="4"/>
       <c r="D15" s="5" t="s">
         <v>8</v>
@@ -985,8 +1266,24 @@
       <c r="H15" s="13" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J15" s="4"/>
+      <c r="K15" s="5">
+        <v>10</v>
+      </c>
+      <c r="L15" s="12" t="s">
+        <v>96</v>
+      </c>
+      <c r="M15" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="N15" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="O15" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C16" s="4"/>
       <c r="D16" s="5" t="s">
         <v>9</v>
@@ -1003,8 +1300,24 @@
       <c r="H16" s="13" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="17" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="J16" s="4"/>
+      <c r="K16" s="5">
+        <v>25</v>
+      </c>
+      <c r="L16" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="M16" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="N16" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="O16" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C17" s="4"/>
       <c r="D17" s="5" t="s">
         <v>10</v>
@@ -1021,8 +1334,24 @@
       <c r="H17" s="13" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="18" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="J17" s="4"/>
+      <c r="K17" s="5">
+        <v>50</v>
+      </c>
+      <c r="L17" s="12" t="s">
+        <v>99</v>
+      </c>
+      <c r="M17" s="12" t="s">
+        <v>100</v>
+      </c>
+      <c r="N17" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="O17" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C18" s="4"/>
       <c r="D18" s="5" t="s">
         <v>11</v>
@@ -1039,8 +1368,24 @@
       <c r="H18" s="13" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="19" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="J18" s="4"/>
+      <c r="K18" s="5">
+        <v>100</v>
+      </c>
+      <c r="L18" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="M18" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="N18" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="O18" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C19" s="4"/>
       <c r="D19" s="5" t="s">
         <v>12</v>
@@ -1057,8 +1402,24 @@
       <c r="H19" s="13" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="20" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="J19" s="4"/>
+      <c r="K19" s="5">
+        <v>250</v>
+      </c>
+      <c r="L19" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="M19" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="N19" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="O19" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C20" s="4"/>
       <c r="D20" s="5" t="s">
         <v>13</v>
@@ -1075,8 +1436,24 @@
       <c r="H20" s="13" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="21" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="J20" s="4"/>
+      <c r="K20" s="5">
+        <v>500</v>
+      </c>
+      <c r="L20" s="12" t="s">
+        <v>104</v>
+      </c>
+      <c r="M20" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="N20" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="O20" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C21" s="7"/>
       <c r="D21" s="8" t="s">
         <v>14</v>
@@ -1093,8 +1470,24 @@
       <c r="H21" s="17" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="22" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="J21" s="7"/>
+      <c r="K21" s="8">
+        <v>1000</v>
+      </c>
+      <c r="L21" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="M21" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="N21" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="O21" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C22" s="1" t="s">
         <v>66</v>
       </c>
@@ -1114,7 +1507,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="23" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C23" s="4"/>
       <c r="D23" s="5" t="s">
         <v>7</v>
@@ -1132,7 +1525,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="24" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C24" s="4"/>
       <c r="D24" s="5" t="s">
         <v>8</v>
@@ -1150,7 +1543,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="25" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C25" s="4"/>
       <c r="D25" s="5" t="s">
         <v>9</v>
@@ -1168,7 +1561,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="26" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C26" s="4"/>
       <c r="D26" s="5" t="s">
         <v>10</v>
@@ -1186,7 +1579,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="27" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C27" s="4"/>
       <c r="D27" s="5" t="s">
         <v>11</v>
@@ -1204,7 +1597,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="28" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C28" s="4"/>
       <c r="D28" s="5" t="s">
         <v>12</v>
@@ -1222,7 +1615,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="29" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C29" s="4"/>
       <c r="D29" s="5" t="s">
         <v>13</v>
@@ -1240,7 +1633,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="30" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C30" s="7"/>
       <c r="D30" s="8" t="s">
         <v>14</v>

</xml_diff>